<commit_message>
Finished off play all function
</commit_message>
<xml_diff>
--- a/Data/stageData1.xlsx
+++ b/Data/stageData1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
   <si>
     <t>stage</t>
   </si>
@@ -220,13 +220,19 @@
   </si>
   <si>
     <t>133.5 km (83 mi)</t>
+  </si>
+  <si>
+    <t>The first stage of the 100th Tour de France was designed to end with a sprint. That's how it panned out but it was anything but a standard finish in Bastia. Ultimately it was a sprinter with a great reputation, Marcel Kittel, who lived up to expectations and claimed the win and the first yellow jersey of the 2013. "This is the greatest day of my life,"he declared at the finish. "This is absolutely something that's outstanding."That was his appraisal after a manic end to the first stage of the Tour to ever be contested in Corsica. The race jury was forced to make quick decisions and originally opt to alter the site of the finish... when the peloton was just eight kilometres away. A bus wedged under the finish structure meant it was not going to be possible to have the sprint end where it had long been planned to be and the commissaires declared that the 3km to go banner would mark the end of the opening stage. But then the bus got unstuck, and with just 2km to go in what was the altered stage, it was back to the original plan: the finish was to be at the finish. This incident, and crashes in the final 12km - that included, amongst other, Alberto Contador and Peter Sagan - will be the talking point on a day when Kittel deserves the accolades. He raced. He won. And he had no idea that there was ever an attempt to amend where the site of the finish was. "I heard my directeur sportif shouting but I didn't understand what he was saying," he confessed. "It was too frantic in the finale."</t>
+  </si>
+  <si>
+    <t>Blurb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +366,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -703,9 +716,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1027,15 +1041,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1054,8 +1068,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1074,8 +1091,11 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1095,7 +1115,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1115,7 +1135,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1135,7 +1155,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1155,7 +1175,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1175,7 +1195,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1195,7 +1215,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1215,7 +1235,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1235,7 +1255,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1255,7 +1275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1275,7 +1295,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1295,7 +1315,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1315,7 +1335,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1335,7 +1355,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1477,5 +1497,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>